<commit_message>
Algunos arreglos en la matriz de riesgos.
</commit_message>
<xml_diff>
--- a/Matriz de Riesgos - Plan de Contingencias/Matriz de Riesgos.xlsx
+++ b/Matriz de Riesgos - Plan de Contingencias/Matriz de Riesgos.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995"/>
@@ -45,9 +45,6 @@
     <t>Robo de equipos del área de servidores o de racks (discos, servidores,  router, switch, modem)</t>
   </si>
   <si>
-    <t>Inundación</t>
-  </si>
-  <si>
     <t>Incendio</t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>Caída temporal del Servidor debido a falla de hardware.</t>
   </si>
   <si>
-    <t>Se cuentan con extinguidores y sistemas de irrigación (con detectores de humo).</t>
-  </si>
-  <si>
-    <t>Se cuenta con generadores eléctricos para cortes prolongados de más de 1 hora.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Se cuenta con firewalls, antivirus, sistemas de monitoreo de entrada y salida de archivos, control de todas la terminales de las sucursales </t>
   </si>
   <si>
@@ -96,10 +87,19 @@
     <t>Los usuarios no tienen privilegios como para realizar modificaciones sobre el sistema operativo. La actividad en la red es monitoreada para detectar posibles actitudes sospechosas, o  futuros ataques internos.</t>
   </si>
   <si>
-    <t>Los servidores estarán ubicados a una altura considerable a salvo de posibles inundaciones.</t>
-  </si>
-  <si>
     <t>Caída de la Base De Datos</t>
+  </si>
+  <si>
+    <t>Se cuentan con extintores y sistemas de irrigación (con detectores de humo).</t>
+  </si>
+  <si>
+    <t>Los servidores estarán ubicados a 1 m. de altura, a salvo de posibles inundaciones. Además la sala cuenta con alcantarillas para desagotar rápidamente cualquier fuga de agua.</t>
+  </si>
+  <si>
+    <t>Inundación de la sala de servidores causada por daños en las cañerías del baño cercano (o baños de pisos superiores)</t>
+  </si>
+  <si>
+    <t>Para cortes de energía de corto tiempo, hay asignadas UPSs para mantener la alimentación de los servidores. Además, se cuenta con generadores eléctricos para cortes prolongados de más de 1 hora.</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -177,6 +177,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -482,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +520,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>5</v>
@@ -531,105 +534,105 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>0.05</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>0.1</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
-        <v>0.09</v>
+        <v>0.4</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>0.17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>0.04</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Arreglos en Matriz de Riesgos y Plan de Contingencias.docx y Matriz de Riesgos.xlsx.
</commit_message>
<xml_diff>
--- a/Matriz de Riesgos - Plan de Contingencias/Matriz de Riesgos.xlsx
+++ b/Matriz de Riesgos - Plan de Contingencias/Matriz de Riesgos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Riesgo</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Robo de equipos del área de servidores o de racks (discos, servidores,  router, switch, modem)</t>
   </si>
   <si>
-    <t>Incendio</t>
-  </si>
-  <si>
-    <t>Corte de energía eléctrica</t>
-  </si>
-  <si>
     <t>Virus informáticos</t>
   </si>
   <si>
@@ -90,16 +84,16 @@
     <t>Caída de la Base De Datos</t>
   </si>
   <si>
-    <t>Se cuentan con extintores y sistemas de irrigación (con detectores de humo).</t>
-  </si>
-  <si>
-    <t>Los servidores estarán ubicados a 1 m. de altura, a salvo de posibles inundaciones. Además la sala cuenta con alcantarillas para desagotar rápidamente cualquier fuga de agua.</t>
-  </si>
-  <si>
     <t>Inundación de la sala de servidores causada por daños en las cañerías del baño cercano (o baños de pisos superiores)</t>
   </si>
   <si>
     <t>Para cortes de energía de corto tiempo, hay asignadas UPSs para mantener la alimentación de los servidores. Además, se cuenta con generadores eléctricos para cortes prolongados de más de 1 hora.</t>
+  </si>
+  <si>
+    <t>Corte de energía eléctrica debido a fallas por parte del proveedor</t>
+  </si>
+  <si>
+    <t>Ubicar los servidires a 1 m. de altura, a salvo de posibles inundaciones. Además equipar la sala con alcantarillas para desagotar rápidamente cualquier fuga de agua.</t>
   </si>
 </sst>
 </file>
@@ -150,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,9 +166,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -483,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D19"/>
+  <dimension ref="A3:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,15 +525,18 @@
         <v>7</v>
       </c>
       <c r="C5" s="2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>26</v>
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>0.05</v>
@@ -551,92 +545,84 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="C8" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="C9" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.17</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>